<commit_message>
Fix statistics to count for all type
</commit_message>
<xml_diff>
--- a/Filatelia_2013.xlsx
+++ b/Filatelia_2013.xlsx
@@ -2677,11 +2677,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="97644928"/>
-        <c:axId val="97646464"/>
+        <c:axId val="177926528"/>
+        <c:axId val="177928064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="97644928"/>
+        <c:axId val="177926528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2690,7 +2690,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97646464"/>
+        <c:crossAx val="177928064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2698,7 +2698,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="97646464"/>
+        <c:axId val="177928064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2709,14 +2709,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97644928"/>
+        <c:crossAx val="177926528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3116,9 +3115,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BM950"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A128" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A156" sqref="A156:XFD156"/>
+      <selection pane="topRight" activeCell="AZ24" sqref="AZ24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -3276,7 +3275,7 @@
       <c r="BH1" s="173"/>
       <c r="BI1" s="174">
         <f>BL5/BL3</f>
-        <v>0.45333333333307263</v>
+        <v>0.47999999999971504</v>
       </c>
       <c r="BJ1" s="175"/>
       <c r="BK1" s="283">
@@ -3415,24 +3414,24 @@
       </c>
       <c r="BH2" s="178">
         <f>(BI3/BD3)</f>
-        <v>0.28257733246998107</v>
+        <v>0.28258364352151583</v>
       </c>
       <c r="BI2" s="179">
         <f>(BH2-AS2)</f>
-        <v>4.0421438366300411E-5</v>
+        <v>4.6732489901057939E-5</v>
       </c>
       <c r="BJ2" s="180"/>
       <c r="BK2" s="60">
         <f>AY3</f>
-        <v>12622</v>
+        <v>12623</v>
       </c>
       <c r="BL2" s="76">
         <f>BK2-AV2</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="BM2" s="54">
         <f>(BK2/AV2)-1</f>
-        <v>1.0310095963201871E-3</v>
+        <v>1.1103180268061674E-3</v>
       </c>
     </row>
     <row r="3" spans="1:65" x14ac:dyDescent="0.2">
@@ -3581,7 +3580,7 @@
       </c>
       <c r="AY3" s="181">
         <f>SUM(AY8:AY190)</f>
-        <v>12622</v>
+        <v>12623</v>
       </c>
       <c r="AZ3" s="182"/>
       <c r="BA3" s="183">
@@ -3598,14 +3597,14 @@
       </c>
       <c r="BE3" s="184">
         <f>BD3/AY3</f>
-        <v>0.25107304706068762</v>
+        <v>0.25105315693575214</v>
       </c>
       <c r="BF3" s="183"/>
       <c r="BG3" s="185"/>
       <c r="BH3" s="186"/>
       <c r="BI3" s="187">
         <f>SUM(BI8:BI190)</f>
-        <v>895.49999999999841</v>
+        <v>895.51999999999839</v>
       </c>
       <c r="BJ3" s="188"/>
       <c r="BK3" s="61">
@@ -3733,15 +3732,15 @@
       <c r="BJ4" s="188"/>
       <c r="BK4" s="86">
         <f>BE3</f>
-        <v>0.25107304706068762</v>
+        <v>0.25105315693575214</v>
       </c>
       <c r="BL4" s="88">
         <f>BK4-AV4</f>
-        <v>-1.9937739803227439E-4</v>
+        <v>-2.1926752296774765E-4</v>
       </c>
       <c r="BM4" s="54">
         <f>(BK4/AV4)-1</f>
-        <v>-7.9347106417171354E-4</v>
+        <v>-8.7262867559023682E-4</v>
       </c>
     </row>
     <row r="5" spans="1:65" x14ac:dyDescent="0.2">
@@ -3832,15 +3831,15 @@
       <c r="BJ5" s="188"/>
       <c r="BK5" s="86">
         <f>BI3</f>
-        <v>895.49999999999841</v>
+        <v>895.51999999999839</v>
       </c>
       <c r="BL5" s="77">
         <f>BK5-AV5</f>
-        <v>0.33999999999980446</v>
+        <v>0.35999999999978627</v>
       </c>
       <c r="BM5" s="54">
         <f>(BK5/AV5)-1</f>
-        <v>3.798203673084366E-4</v>
+        <v>4.0216274185600476E-4</v>
       </c>
     </row>
     <row r="6" spans="1:65" s="75" customFormat="1" x14ac:dyDescent="0.2">
@@ -3958,7 +3957,7 @@
       <c r="AX6" s="74"/>
       <c r="AY6" s="189">
         <f>AY3-AJ3</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AZ6" s="190" t="e">
         <f>AY6/AW2-1</f>
@@ -3982,14 +3981,14 @@
       </c>
       <c r="BE6" s="194">
         <f>BE3-AR3</f>
-        <v>0.25107304706068762</v>
+        <v>0.25105315693575214</v>
       </c>
       <c r="BF6" s="195"/>
       <c r="BG6" s="196"/>
       <c r="BH6" s="197"/>
       <c r="BI6" s="198">
         <f>BI3-AU3</f>
-        <v>895.49999999999841</v>
+        <v>895.51999999999839</v>
       </c>
       <c r="BJ6" s="199"/>
       <c r="BK6" s="74"/>
@@ -18587,8 +18586,8 @@
       <c r="BM79" s="59"/>
     </row>
     <row r="80" spans="1:65" x14ac:dyDescent="0.2">
-      <c r="A80" s="103" t="s">
-        <v>22</v>
+      <c r="A80" s="99" t="s">
+        <v>51</v>
       </c>
       <c r="B80" s="104"/>
       <c r="C80" s="15">
@@ -18606,40 +18605,40 @@
         <v>0</v>
       </c>
       <c r="G80" s="18">
-        <v>104</v>
+        <v>128</v>
       </c>
       <c r="H80" s="21"/>
       <c r="I80" s="41">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="J80" s="42">
         <f>I80-C80</f>
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="K80" s="43">
-        <v>21.65</v>
+        <v>3</v>
       </c>
       <c r="L80" s="44">
         <f>K80-D80</f>
-        <v>21.65</v>
+        <v>3</v>
       </c>
       <c r="M80" s="43">
         <f>K80*0.2</f>
-        <v>4.33</v>
+        <v>0.60000000000000009</v>
       </c>
       <c r="N80" s="45">
         <f>IF(I80&gt;0,K80/I80,0)</f>
-        <v>2.4055555555555554</v>
+        <v>3</v>
       </c>
       <c r="O80" s="46">
-        <v>56</v>
+        <v>128</v>
       </c>
       <c r="P80" s="42">
         <f>(O80-G80)*-1</f>
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="Q80" s="47">
-        <v>0.15</v>
+        <v>0.02</v>
       </c>
       <c r="R80" s="59"/>
       <c r="S80" s="59"/>
@@ -18649,44 +18648,44 @@
       </c>
       <c r="V80" s="261">
         <f>U80-I80</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="W80" s="262">
-        <v>22.65</v>
+        <v>7.9</v>
       </c>
       <c r="X80" s="263">
         <f>W80-K80</f>
-        <v>1</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="Y80" s="264">
         <f>IF(K80&lt;&gt;0,(W80/K80)-1,"NEW")</f>
-        <v>4.6189376443418029E-2</v>
+        <v>1.6333333333333333</v>
       </c>
       <c r="Z80" s="262">
         <f>W80*0.2</f>
-        <v>4.53</v>
+        <v>1.58</v>
       </c>
       <c r="AA80" s="265">
         <f>IF(U80&gt;0,W80/U80,0)</f>
-        <v>2.5166666666666666</v>
+        <v>0.87777777777777777</v>
       </c>
       <c r="AB80" s="266">
         <f>AA80-N80</f>
-        <v>0.11111111111111116</v>
+        <v>-2.1222222222222222</v>
       </c>
       <c r="AC80" s="267">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="AD80" s="268">
         <f>(AC80-O80)*-1</f>
-        <v>-16</v>
+        <v>53</v>
       </c>
       <c r="AE80" s="269">
         <v>0.16</v>
       </c>
       <c r="AF80" s="270">
         <f>AE80/W80</f>
-        <v>7.064017660044151E-3</v>
+        <v>2.0253164556962026E-2</v>
       </c>
       <c r="AG80" s="59"/>
       <c r="AH80" s="59"/>
@@ -18696,14 +18695,14 @@
       </c>
       <c r="AK80" s="323">
         <f>AJ80-X80</f>
-        <v>8</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="AL80" s="324">
-        <v>22.65</v>
+        <v>7.9</v>
       </c>
       <c r="AM80" s="325">
         <f>AL80-Z80</f>
-        <v>18.119999999999997</v>
+        <v>6.32</v>
       </c>
       <c r="AN80" s="326">
         <f>IF(Z80&lt;&gt;0,(AL80/W80)-1,"NEW")</f>
@@ -18711,42 +18710,42 @@
       </c>
       <c r="AO80" s="324">
         <f>AL80*0.2</f>
-        <v>4.53</v>
+        <v>1.58</v>
       </c>
       <c r="AP80" s="327">
         <f>IF(AJ80&gt;0,AL80/AJ80,0)</f>
-        <v>2.5166666666666666</v>
+        <v>0.87777777777777777</v>
       </c>
       <c r="AQ80" s="328">
         <f>AP80-AC80</f>
-        <v>-69.483333333333334</v>
+        <v>-74.12222222222222</v>
       </c>
       <c r="AR80" s="329">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="AS80" s="330">
         <f>(AR80-AD80)*-1</f>
-        <v>-88</v>
+        <v>-22</v>
       </c>
       <c r="AT80" s="331">
         <v>0.16</v>
       </c>
       <c r="AU80" s="332">
         <f>AT80/AL80</f>
-        <v>7.064017660044151E-3</v>
+        <v>2.0253164556962026E-2</v>
       </c>
       <c r="AV80" s="59"/>
       <c r="AW80" s="59"/>
       <c r="AX80" s="59"/>
       <c r="AY80" s="205">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AZ80" s="206">
         <f>AY80-AJ80</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA80" s="207">
-        <v>22.65</v>
+        <v>7.9</v>
       </c>
       <c r="BB80" s="208">
         <f>BA80-AL80</f>
@@ -18758,37 +18757,37 @@
       </c>
       <c r="BD80" s="207">
         <f>BA80*0.2</f>
-        <v>4.53</v>
+        <v>1.58</v>
       </c>
       <c r="BE80" s="210">
         <f>IF(AY80&gt;0,BA80/AY80,0)</f>
-        <v>2.5166666666666666</v>
+        <v>0.79</v>
       </c>
       <c r="BF80" s="211">
         <f>BE80-AP80</f>
-        <v>0</v>
+        <v>-8.7777777777777732E-2</v>
       </c>
       <c r="BG80" s="212">
         <v>73</v>
       </c>
       <c r="BH80" s="213">
         <f>(BG80-AR80)*-1</f>
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="BI80" s="214">
-        <v>0.16</v>
+        <v>0.18</v>
       </c>
       <c r="BJ80" s="215">
         <f>BI80/BA80</f>
-        <v>7.064017660044151E-3</v>
+        <v>2.2784810126582275E-2</v>
       </c>
       <c r="BK80" s="59"/>
       <c r="BL80" s="59"/>
       <c r="BM80" s="59"/>
     </row>
     <row r="81" spans="1:65" x14ac:dyDescent="0.2">
-      <c r="A81" s="99" t="s">
-        <v>78</v>
+      <c r="A81" s="103" t="s">
+        <v>22</v>
       </c>
       <c r="B81" s="104"/>
       <c r="C81" s="15">
@@ -18806,40 +18805,40 @@
         <v>0</v>
       </c>
       <c r="G81" s="18">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="H81" s="21"/>
       <c r="I81" s="41">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="J81" s="42">
         <f>I81-C81</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="K81" s="43">
-        <v>0.4</v>
+        <v>21.65</v>
       </c>
       <c r="L81" s="44">
         <f>K81-D81</f>
-        <v>0.4</v>
+        <v>21.65</v>
       </c>
       <c r="M81" s="43">
         <f>K81*0.2</f>
-        <v>8.0000000000000016E-2</v>
+        <v>4.33</v>
       </c>
       <c r="N81" s="45">
         <f>IF(I81&gt;0,K81/I81,0)</f>
-        <v>0.2</v>
+        <v>2.4055555555555554</v>
       </c>
       <c r="O81" s="46">
-        <v>106</v>
+        <v>56</v>
       </c>
       <c r="P81" s="42">
         <f>(O81-G81)*-1</f>
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="Q81" s="47">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="R81" s="59"/>
       <c r="S81" s="59"/>
@@ -18849,44 +18848,44 @@
       </c>
       <c r="V81" s="261">
         <f>U81-I81</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="W81" s="262">
-        <v>11.35</v>
+        <v>22.65</v>
       </c>
       <c r="X81" s="263">
         <f>W81-K81</f>
-        <v>10.95</v>
+        <v>1</v>
       </c>
       <c r="Y81" s="264">
         <f>IF(K81&lt;&gt;0,(W81/K81)-1,"NEW")</f>
-        <v>27.374999999999996</v>
+        <v>4.6189376443418029E-2</v>
       </c>
       <c r="Z81" s="262">
         <f>W81*0.2</f>
-        <v>2.27</v>
+        <v>4.53</v>
       </c>
       <c r="AA81" s="265">
         <f>IF(U81&gt;0,W81/U81,0)</f>
-        <v>1.2611111111111111</v>
+        <v>2.5166666666666666</v>
       </c>
       <c r="AB81" s="266">
         <f>AA81-N81</f>
-        <v>1.0611111111111111</v>
+        <v>0.11111111111111116</v>
       </c>
       <c r="AC81" s="267">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AD81" s="268">
         <f>(AC81-O81)*-1</f>
-        <v>33</v>
+        <v>-16</v>
       </c>
       <c r="AE81" s="269">
-        <v>2.02</v>
+        <v>0.16</v>
       </c>
       <c r="AF81" s="270">
         <f>AE81/W81</f>
-        <v>0.17797356828193833</v>
+        <v>7.064017660044151E-3</v>
       </c>
       <c r="AG81" s="59"/>
       <c r="AH81" s="59"/>
@@ -18896,14 +18895,14 @@
       </c>
       <c r="AK81" s="323">
         <f>AJ81-X81</f>
-        <v>-1.9499999999999993</v>
+        <v>8</v>
       </c>
       <c r="AL81" s="324">
-        <v>11.35</v>
+        <v>22.65</v>
       </c>
       <c r="AM81" s="325">
         <f>AL81-Z81</f>
-        <v>9.08</v>
+        <v>18.119999999999997</v>
       </c>
       <c r="AN81" s="326">
         <f>IF(Z81&lt;&gt;0,(AL81/W81)-1,"NEW")</f>
@@ -18911,29 +18910,29 @@
       </c>
       <c r="AO81" s="324">
         <f>AL81*0.2</f>
-        <v>2.27</v>
+        <v>4.53</v>
       </c>
       <c r="AP81" s="327">
         <f>IF(AJ81&gt;0,AL81/AJ81,0)</f>
-        <v>1.2611111111111111</v>
+        <v>2.5166666666666666</v>
       </c>
       <c r="AQ81" s="328">
         <f>AP81-AC81</f>
-        <v>-71.738888888888894</v>
+        <v>-69.483333333333334</v>
       </c>
       <c r="AR81" s="329">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AS81" s="330">
         <f>(AR81-AD81)*-1</f>
-        <v>-40</v>
+        <v>-88</v>
       </c>
       <c r="AT81" s="331">
-        <v>2.02</v>
+        <v>0.16</v>
       </c>
       <c r="AU81" s="332">
         <f>AT81/AL81</f>
-        <v>0.17797356828193833</v>
+        <v>7.064017660044151E-3</v>
       </c>
       <c r="AV81" s="59"/>
       <c r="AW81" s="59"/>
@@ -18946,7 +18945,7 @@
         <v>0</v>
       </c>
       <c r="BA81" s="207">
-        <v>11.35</v>
+        <v>22.65</v>
       </c>
       <c r="BB81" s="208">
         <f>BA81-AL81</f>
@@ -18958,11 +18957,11 @@
       </c>
       <c r="BD81" s="207">
         <f>BA81*0.2</f>
-        <v>2.27</v>
+        <v>4.53</v>
       </c>
       <c r="BE81" s="210">
         <f>IF(AY81&gt;0,BA81/AY81,0)</f>
-        <v>1.2611111111111111</v>
+        <v>2.5166666666666666</v>
       </c>
       <c r="BF81" s="211">
         <f>BE81-AP81</f>
@@ -18973,14 +18972,14 @@
       </c>
       <c r="BH81" s="213">
         <f>(BG81-AR81)*-1</f>
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="BI81" s="214">
-        <v>2.02</v>
+        <v>0.16</v>
       </c>
       <c r="BJ81" s="215">
         <f>BI81/BA81</f>
-        <v>0.17797356828193833</v>
+        <v>7.064017660044151E-3</v>
       </c>
       <c r="BK81" s="59"/>
       <c r="BL81" s="59"/>
@@ -18988,59 +18987,59 @@
     </row>
     <row r="82" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A82" s="99" t="s">
-        <v>64</v>
-      </c>
-      <c r="B82" s="104">
-        <v>174</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="B82" s="104"/>
       <c r="C82" s="15">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D82" s="56">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="E82" s="56">
         <f>D82*0.2</f>
-        <v>0.24</v>
+        <v>0</v>
       </c>
       <c r="F82" s="58">
         <f>IF(C82&gt;0,D82/C82,0)</f>
-        <v>0.39999999999999997</v>
+        <v>0</v>
       </c>
       <c r="G82" s="18">
-        <v>51</v>
+        <v>119</v>
       </c>
       <c r="H82" s="21"/>
       <c r="I82" s="41">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J82" s="42">
         <f>I82-C82</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K82" s="43">
-        <v>1.4</v>
+        <v>0.4</v>
       </c>
       <c r="L82" s="44">
         <f>K82-D82</f>
-        <v>0.19999999999999996</v>
+        <v>0.4</v>
       </c>
       <c r="M82" s="43">
         <f>K82*0.2</f>
-        <v>0.27999999999999997</v>
+        <v>8.0000000000000016E-2</v>
       </c>
       <c r="N82" s="45">
         <f>IF(I82&gt;0,K82/I82,0)</f>
-        <v>0.35</v>
+        <v>0.2</v>
       </c>
       <c r="O82" s="46">
-        <v>77</v>
+        <v>106</v>
       </c>
       <c r="P82" s="42">
         <f>(O82-G82)*-1</f>
-        <v>-26</v>
-      </c>
-      <c r="Q82" s="47"/>
+        <v>13</v>
+      </c>
+      <c r="Q82" s="47">
+        <v>0.2</v>
+      </c>
       <c r="R82" s="59"/>
       <c r="S82" s="59"/>
       <c r="T82" s="59"/>
@@ -19049,44 +19048,44 @@
       </c>
       <c r="V82" s="261">
         <f>U82-I82</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="W82" s="262">
-        <v>8.4499999999999993</v>
+        <v>11.35</v>
       </c>
       <c r="X82" s="263">
         <f>W82-K82</f>
-        <v>7.0499999999999989</v>
+        <v>10.95</v>
       </c>
       <c r="Y82" s="264">
         <f>IF(K82&lt;&gt;0,(W82/K82)-1,"NEW")</f>
-        <v>5.0357142857142856</v>
+        <v>27.374999999999996</v>
       </c>
       <c r="Z82" s="262">
         <f>W82*0.2</f>
-        <v>1.69</v>
+        <v>2.27</v>
       </c>
       <c r="AA82" s="265">
         <f>IF(U82&gt;0,W82/U82,0)</f>
-        <v>0.93888888888888877</v>
+        <v>1.2611111111111111</v>
       </c>
       <c r="AB82" s="266">
         <f>AA82-N82</f>
-        <v>0.5888888888888888</v>
+        <v>1.0611111111111111</v>
       </c>
       <c r="AC82" s="267">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AD82" s="268">
         <f>(AC82-O82)*-1</f>
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="AE82" s="269">
-        <v>0.06</v>
+        <v>2.02</v>
       </c>
       <c r="AF82" s="270">
         <f>AE82/W82</f>
-        <v>7.1005917159763319E-3</v>
+        <v>0.17797356828193833</v>
       </c>
       <c r="AG82" s="59"/>
       <c r="AH82" s="59"/>
@@ -19096,14 +19095,14 @@
       </c>
       <c r="AK82" s="323">
         <f>AJ82-X82</f>
-        <v>1.9500000000000011</v>
+        <v>-1.9499999999999993</v>
       </c>
       <c r="AL82" s="324">
-        <v>8.4499999999999993</v>
+        <v>11.35</v>
       </c>
       <c r="AM82" s="325">
         <f>AL82-Z82</f>
-        <v>6.76</v>
+        <v>9.08</v>
       </c>
       <c r="AN82" s="326">
         <f>IF(Z82&lt;&gt;0,(AL82/W82)-1,"NEW")</f>
@@ -19111,29 +19110,29 @@
       </c>
       <c r="AO82" s="324">
         <f>AL82*0.2</f>
-        <v>1.69</v>
+        <v>2.27</v>
       </c>
       <c r="AP82" s="327">
         <f>IF(AJ82&gt;0,AL82/AJ82,0)</f>
-        <v>0.93888888888888877</v>
+        <v>1.2611111111111111</v>
       </c>
       <c r="AQ82" s="328">
         <f>AP82-AC82</f>
-        <v>-73.061111111111117</v>
+        <v>-71.738888888888894</v>
       </c>
       <c r="AR82" s="329">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AS82" s="330">
         <f>(AR82-AD82)*-1</f>
-        <v>-71</v>
+        <v>-40</v>
       </c>
       <c r="AT82" s="331">
-        <v>0.06</v>
+        <v>2.02</v>
       </c>
       <c r="AU82" s="332">
         <f>AT82/AL82</f>
-        <v>7.1005917159763319E-3</v>
+        <v>0.17797356828193833</v>
       </c>
       <c r="AV82" s="59"/>
       <c r="AW82" s="59"/>
@@ -19146,7 +19145,7 @@
         <v>0</v>
       </c>
       <c r="BA82" s="207">
-        <v>8.4499999999999993</v>
+        <v>11.35</v>
       </c>
       <c r="BB82" s="208">
         <f>BA82-AL82</f>
@@ -19158,11 +19157,11 @@
       </c>
       <c r="BD82" s="207">
         <f>BA82*0.2</f>
-        <v>1.69</v>
+        <v>2.27</v>
       </c>
       <c r="BE82" s="210">
         <f>IF(AY82&gt;0,BA82/AY82,0)</f>
-        <v>0.93888888888888877</v>
+        <v>1.2611111111111111</v>
       </c>
       <c r="BF82" s="211">
         <f>BE82-AP82</f>
@@ -19173,14 +19172,14 @@
       </c>
       <c r="BH82" s="213">
         <f>(BG82-AR82)*-1</f>
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="BI82" s="214">
-        <v>0.06</v>
+        <v>2.02</v>
       </c>
       <c r="BJ82" s="215">
         <f>BI82/BA82</f>
-        <v>7.1005917159763319E-3</v>
+        <v>0.17797356828193833</v>
       </c>
       <c r="BK82" s="59"/>
       <c r="BL82" s="59"/>
@@ -19188,59 +19187,59 @@
     </row>
     <row r="83" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A83" s="99" t="s">
-        <v>51</v>
-      </c>
-      <c r="B83" s="104"/>
+        <v>64</v>
+      </c>
+      <c r="B83" s="104">
+        <v>174</v>
+      </c>
       <c r="C83" s="15">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D83" s="56">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="E83" s="56">
         <f>D83*0.2</f>
-        <v>0</v>
+        <v>0.24</v>
       </c>
       <c r="F83" s="58">
         <f>IF(C83&gt;0,D83/C83,0)</f>
-        <v>0</v>
+        <v>0.39999999999999997</v>
       </c>
       <c r="G83" s="18">
-        <v>128</v>
+        <v>51</v>
       </c>
       <c r="H83" s="21"/>
       <c r="I83" s="41">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J83" s="42">
         <f>I83-C83</f>
         <v>1</v>
       </c>
       <c r="K83" s="43">
-        <v>3</v>
+        <v>1.4</v>
       </c>
       <c r="L83" s="44">
         <f>K83-D83</f>
-        <v>3</v>
+        <v>0.19999999999999996</v>
       </c>
       <c r="M83" s="43">
         <f>K83*0.2</f>
-        <v>0.60000000000000009</v>
+        <v>0.27999999999999997</v>
       </c>
       <c r="N83" s="45">
         <f>IF(I83&gt;0,K83/I83,0)</f>
-        <v>3</v>
+        <v>0.35</v>
       </c>
       <c r="O83" s="46">
-        <v>128</v>
+        <v>77</v>
       </c>
       <c r="P83" s="42">
         <f>(O83-G83)*-1</f>
-        <v>0</v>
-      </c>
-      <c r="Q83" s="47">
-        <v>0.02</v>
-      </c>
+        <v>-26</v>
+      </c>
+      <c r="Q83" s="47"/>
       <c r="R83" s="59"/>
       <c r="S83" s="59"/>
       <c r="T83" s="59"/>
@@ -19249,44 +19248,44 @@
       </c>
       <c r="V83" s="261">
         <f>U83-I83</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="W83" s="262">
-        <v>7.9</v>
+        <v>8.4499999999999993</v>
       </c>
       <c r="X83" s="263">
         <f>W83-K83</f>
-        <v>4.9000000000000004</v>
+        <v>7.0499999999999989</v>
       </c>
       <c r="Y83" s="264">
         <f>IF(K83&lt;&gt;0,(W83/K83)-1,"NEW")</f>
-        <v>1.6333333333333333</v>
+        <v>5.0357142857142856</v>
       </c>
       <c r="Z83" s="262">
         <f>W83*0.2</f>
-        <v>1.58</v>
+        <v>1.69</v>
       </c>
       <c r="AA83" s="265">
         <f>IF(U83&gt;0,W83/U83,0)</f>
-        <v>0.87777777777777777</v>
+        <v>0.93888888888888877</v>
       </c>
       <c r="AB83" s="266">
         <f>AA83-N83</f>
-        <v>-2.1222222222222222</v>
+        <v>0.5888888888888888</v>
       </c>
       <c r="AC83" s="267">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AD83" s="268">
         <f>(AC83-O83)*-1</f>
-        <v>53</v>
+        <v>3</v>
       </c>
       <c r="AE83" s="269">
-        <v>0.16</v>
+        <v>0.06</v>
       </c>
       <c r="AF83" s="270">
         <f>AE83/W83</f>
-        <v>2.0253164556962026E-2</v>
+        <v>7.1005917159763319E-3</v>
       </c>
       <c r="AG83" s="59"/>
       <c r="AH83" s="59"/>
@@ -19296,14 +19295,14 @@
       </c>
       <c r="AK83" s="323">
         <f>AJ83-X83</f>
-        <v>4.0999999999999996</v>
+        <v>1.9500000000000011</v>
       </c>
       <c r="AL83" s="324">
-        <v>7.9</v>
+        <v>8.4499999999999993</v>
       </c>
       <c r="AM83" s="325">
         <f>AL83-Z83</f>
-        <v>6.32</v>
+        <v>6.76</v>
       </c>
       <c r="AN83" s="326">
         <f>IF(Z83&lt;&gt;0,(AL83/W83)-1,"NEW")</f>
@@ -19311,29 +19310,29 @@
       </c>
       <c r="AO83" s="324">
         <f>AL83*0.2</f>
-        <v>1.58</v>
+        <v>1.69</v>
       </c>
       <c r="AP83" s="327">
         <f>IF(AJ83&gt;0,AL83/AJ83,0)</f>
-        <v>0.87777777777777777</v>
+        <v>0.93888888888888877</v>
       </c>
       <c r="AQ83" s="328">
         <f>AP83-AC83</f>
-        <v>-74.12222222222222</v>
+        <v>-73.061111111111117</v>
       </c>
       <c r="AR83" s="329">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AS83" s="330">
         <f>(AR83-AD83)*-1</f>
-        <v>-22</v>
+        <v>-71</v>
       </c>
       <c r="AT83" s="331">
-        <v>0.16</v>
+        <v>0.06</v>
       </c>
       <c r="AU83" s="332">
         <f>AT83/AL83</f>
-        <v>2.0253164556962026E-2</v>
+        <v>7.1005917159763319E-3</v>
       </c>
       <c r="AV83" s="59"/>
       <c r="AW83" s="59"/>
@@ -19346,7 +19345,7 @@
         <v>0</v>
       </c>
       <c r="BA83" s="207">
-        <v>7.9</v>
+        <v>8.4499999999999993</v>
       </c>
       <c r="BB83" s="208">
         <f>BA83-AL83</f>
@@ -19358,11 +19357,11 @@
       </c>
       <c r="BD83" s="207">
         <f>BA83*0.2</f>
-        <v>1.58</v>
+        <v>1.69</v>
       </c>
       <c r="BE83" s="210">
         <f>IF(AY83&gt;0,BA83/AY83,0)</f>
-        <v>0.87777777777777777</v>
+        <v>0.93888888888888877</v>
       </c>
       <c r="BF83" s="211">
         <f>BE83-AP83</f>
@@ -19373,14 +19372,14 @@
       </c>
       <c r="BH83" s="213">
         <f>(BG83-AR83)*-1</f>
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="BI83" s="214">
-        <v>0.16</v>
+        <v>0.06</v>
       </c>
       <c r="BJ83" s="215">
         <f>BI83/BA83</f>
-        <v>2.0253164556962026E-2</v>
+        <v>7.1005917159763319E-3</v>
       </c>
       <c r="BK83" s="59"/>
       <c r="BL83" s="59"/>

</xml_diff>